<commit_message>
Updating the EF ontology
</commit_message>
<xml_diff>
--- a/dev/ontologies.xlsx
+++ b/dev/ontologies.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlee9\Documents\GitHub\DOE_SDI\flexibility_ontology\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76D30129-6FDB-4373-B8D0-22E5AB0409B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E89C3B2-4B5A-488B-9512-FA136400E2CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2100" xr2:uid="{8873C2BF-8AB8-412F-B2BC-36F27E750B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,8 +110,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{3C686E50-78B6-45F1-B892-79AA512A7D86}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -420,7 +451,7 @@
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update the EF ontology, added new existing ontologies
</commit_message>
<xml_diff>
--- a/dev/ontologies.xlsx
+++ b/dev/ontologies.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlee9\Documents\GitHub\DOE_SDI\flexibility_ontology\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E89C3B2-4B5A-488B-9512-FA136400E2CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0A612F-DC46-4CC5-89B8-2380D1EADDAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2100" xr2:uid="{8873C2BF-8AB8-412F-B2BC-36F27E750B64}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2100" activeTab="1" xr2:uid="{8873C2BF-8AB8-412F-B2BC-36F27E750B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>building information</t>
   </si>
@@ -58,13 +59,94 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Ontology Name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Semantic Technology</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Demand Response</t>
+  </si>
+  <si>
+    <t>SAREF4</t>
+  </si>
+  <si>
+    <t>ThinkHome</t>
+  </si>
+  <si>
+    <t>OEMA</t>
+  </si>
+  <si>
+    <t>Building Topology</t>
+  </si>
+  <si>
+    <t>Brick</t>
+  </si>
+  <si>
+    <t>Building Geometry</t>
+  </si>
+  <si>
+    <t>EM-KPI</t>
+  </si>
+  <si>
+    <t>Metrics/KPIs</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Building Construction</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>KPI-Ont</t>
+  </si>
+  <si>
+    <t>Distributed Energy Resources</t>
+  </si>
+  <si>
+    <t>obXML</t>
+  </si>
+  <si>
+    <t>IFC4</t>
+  </si>
+  <si>
+    <t>End-use System</t>
+  </si>
+  <si>
+    <t>Sensor/ Sensor Network</t>
+  </si>
+  <si>
+    <t>OpenADR</t>
+  </si>
+  <si>
+    <t>Occupancy &amp; Behavior</t>
+  </si>
+  <si>
+    <t>DigitalBuildings</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>DogOnt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +162,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -97,14 +187,193 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -450,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83073FF2-E4A6-4C89-BF81-8BBFDB9347AE}">
   <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,4 +773,325 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144E5BAF-562C-4981-889C-996E54C27DA0}">
+  <dimension ref="B1:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="11" width="11.77734375" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="2:17" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="8"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="5"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>